<commit_message>
Changes in Prahalad local
</commit_message>
<xml_diff>
--- a/Data Files/TestDataFile.xlsx
+++ b/Data Files/TestDataFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Katalon Studio\Kraft_Working\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD61472-C78B-45BE-98B7-E46253F6FA1D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA87EB0-6FCD-4B60-9DA4-FF641B73563B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" tabRatio="714" activeTab="5" xr2:uid="{D4F270EC-5AE8-4120-82CE-49432D331804}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" tabRatio="714" activeTab="3" xr2:uid="{D4F270EC-5AE8-4120-82CE-49432D331804}"/>
   </bookViews>
   <sheets>
     <sheet name="LOGIN" sheetId="1" r:id="rId1"/>
@@ -89,9 +89,6 @@
     <t>UNITS</t>
   </si>
   <si>
-    <t>L22 6-7z Mixed Pasta Salads 12 $13.68</t>
-  </si>
-  <si>
     <t>ADD_NEW</t>
   </si>
   <si>
@@ -243,6 +240,9 @@
   </si>
   <si>
     <t>.08z FS Crystal Light On the Go $25.21</t>
+  </si>
+  <si>
+    <t>13z Velveeta Bowls $32.52</t>
   </si>
 </sst>
 </file>
@@ -746,13 +746,13 @@
         <v>5</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -772,39 +772,39 @@
         <v>14</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F3" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F4" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F5" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F6" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -824,18 +824,18 @@
         <v>14</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G8" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -848,8 +848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE2F7406-B77D-4F70-A3D8-0D67A8563A67}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,22 +888,22 @@
         <v>18</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="J1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -920,25 +920,25 @@
         <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="F2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -983,58 +983,58 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="F1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="R1" s="5" t="s">
-        <v>36</v>
-      </c>
       <c r="S1" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -1042,13 +1042,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="I2" s="3">
         <v>1</v>
@@ -1072,10 +1072,10 @@
         <v>1</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -1083,13 +1083,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="I3" s="3">
         <v>1</v>
@@ -1113,10 +1113,10 @@
         <v>4</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1129,7 +1129,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FD16D48-E1BF-47ED-A849-2E712965AECD}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -1159,13 +1159,13 @@
         <v>6</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="G1" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1182,7 +1182,7 @@
         <v>13</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1190,7 +1190,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>